<commit_message>
Working? monte carlo tree search
</commit_message>
<xml_diff>
--- a/test/assets/abilities.xlsx
+++ b/test/assets/abilities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ran Liu\PycharmProjects\keybind_generator\test\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BEF210-DC6F-49CC-9FCE-FE93436FA7F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893A1E9B-6E1A-49F8-BAA8-6D29E2FAEEF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1755" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6683194F-2724-4542-99E4-27A65288EC1D}"/>
+    <workbookView xWindow="28680" yWindow="-1755" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{6683194F-2724-4542-99E4-27A65288EC1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Key Layout" sheetId="6" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="232">
   <si>
     <t>Ability Name</t>
   </si>
@@ -389,9 +389,6 @@
     <t>Zaros Godsword</t>
   </si>
   <si>
-    <t>Guthix Staff&gt;Special Attack&gt;Wand Switch&gt;Orb Switch</t>
-  </si>
-  <si>
     <t>Ice Barrage&gt;Detonate&gt;Tsunami</t>
   </si>
   <si>
@@ -714,6 +711,27 @@
   </si>
   <si>
     <t>Shift+B</t>
+  </si>
+  <si>
+    <t>Planted Feet Switch&gt;Ring of Vigour&gt;Sunshine</t>
+  </si>
+  <si>
+    <t>Blood Barrage&gt;Wand Switch&gt;Orb Switch</t>
+  </si>
+  <si>
+    <t>Ice Barrage&gt;Guthix Staff&gt;Special Attack&gt;Wand Switch&gt;Orb Switch</t>
+  </si>
+  <si>
+    <t>Blood Barrage&gt;Guthix Staff&gt;Special Attack&gt;Wand Switch&gt;Orb Switch</t>
+  </si>
+  <si>
+    <t>Ice Barrage&gt;Wand Switch&gt;Orb Switch</t>
+  </si>
+  <si>
+    <t>Eat Food&gt;Super Restore Potion</t>
+  </si>
+  <si>
+    <t>Eat Food&gt;Replenishment Potion</t>
   </si>
 </sst>
 </file>
@@ -1112,42 +1130,42 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F2" s="5">
         <v>2</v>
@@ -1158,10 +1176,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F3" s="5">
         <v>1</v>
@@ -1172,10 +1190,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F4" s="5">
         <v>1</v>
@@ -1184,7 +1202,7 @@
         <v>1.5</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J4" s="5">
         <v>4</v>
@@ -1192,10 +1210,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F5" s="5">
         <v>1.5</v>
@@ -1206,10 +1224,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F6" s="5">
         <v>1.5</v>
@@ -1218,7 +1236,7 @@
         <v>2.5</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J6" s="5">
         <v>4</v>
@@ -1226,10 +1244,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F7" s="5">
         <v>1.5</v>
@@ -1238,7 +1256,7 @@
         <v>2.5</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J7" s="5">
         <v>8</v>
@@ -1246,10 +1264,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F8" s="5">
         <v>1.8</v>
@@ -1260,10 +1278,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F9" s="5">
         <v>1.8</v>
@@ -1272,7 +1290,7 @@
         <v>3.5</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J9" s="5">
         <v>4</v>
@@ -1280,10 +1298,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F10" s="5">
         <v>1.8</v>
@@ -1292,7 +1310,7 @@
         <v>3.5</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J10" s="5">
         <v>8</v>
@@ -1300,10 +1318,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F11" s="5">
         <v>2</v>
@@ -1314,10 +1332,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F12" s="5">
         <v>2</v>
@@ -1326,7 +1344,7 @@
         <v>4.5</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J12" s="5">
         <v>4</v>
@@ -1334,10 +1352,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F13" s="5">
         <v>2</v>
@@ -1346,7 +1364,7 @@
         <v>4.5</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J13" s="5">
         <v>8</v>
@@ -1362,8 +1380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C60286-EF72-402C-B298-6B64A6B4C92A}">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>74</v>
@@ -1643,7 +1661,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1654,7 +1672,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -2232,10 +2250,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9A92560-C1D4-4ABC-88FC-7C94D8DEB9F1}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2251,7 +2269,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>112</v>
@@ -2273,7 +2291,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2342,7 +2360,7 @@
         <v>105</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
         <v>76</v>
@@ -2353,7 +2371,7 @@
         <v>106</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
         <v>76</v>
@@ -2364,7 +2382,7 @@
         <v>107</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
         <v>76</v>
@@ -2375,7 +2393,7 @@
         <v>108</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
         <v>76</v>
@@ -2386,7 +2404,7 @@
         <v>109</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
         <v>76</v>
@@ -2397,7 +2415,7 @@
         <v>110</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
         <v>76</v>
@@ -2405,7 +2423,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>228</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2416,7 +2434,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>124</v>
+        <v>227</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2427,7 +2445,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2438,7 +2456,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2449,10 +2467,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
         <v>76</v>
@@ -2460,7 +2478,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -2471,10 +2489,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
         <v>76</v>
@@ -2482,7 +2500,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2493,7 +2511,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -2504,7 +2522,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2515,12 +2533,78 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>225</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>226</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>229</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>230</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>231</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2533,7 +2617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D31F1635-B516-4288-95EF-EB4DDEE5147E}">
   <dimension ref="A1:B77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2548,7 +2632,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2556,7 +2640,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2564,7 +2648,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2580,7 +2664,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2588,7 +2672,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2596,7 +2680,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2604,7 +2688,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2612,7 +2696,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2620,7 +2704,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2628,7 +2712,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2636,7 +2720,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2644,7 +2728,7 @@
         <v>17</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2652,7 +2736,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2660,7 +2744,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2668,7 +2752,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2676,7 +2760,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2684,7 +2768,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2692,7 +2776,7 @@
         <v>22</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2700,7 +2784,7 @@
         <v>23</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2708,7 +2792,7 @@
         <v>24</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2716,7 +2800,7 @@
         <v>25</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2724,7 +2808,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2732,23 +2816,23 @@
         <v>27</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2756,7 +2840,7 @@
         <v>28</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2764,7 +2848,7 @@
         <v>29</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2772,7 +2856,7 @@
         <v>30</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2780,7 +2864,7 @@
         <v>31</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2788,7 +2872,7 @@
         <v>32</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2796,7 +2880,7 @@
         <v>33</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2804,7 +2888,7 @@
         <v>34</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2812,7 +2896,7 @@
         <v>35</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2820,7 +2904,7 @@
         <v>36</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -2828,7 +2912,7 @@
         <v>87</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2836,7 +2920,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2844,7 +2928,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2852,7 +2936,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2860,7 +2944,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2868,7 +2952,7 @@
         <v>71</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2876,7 +2960,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2884,7 +2968,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2892,7 +2976,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2900,7 +2984,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2908,7 +2992,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2916,7 +3000,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2924,7 +3008,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2932,7 +3016,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2940,7 +3024,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2948,7 +3032,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2956,7 +3040,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2964,7 +3048,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2972,7 +3056,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2980,7 +3064,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2988,7 +3072,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2996,7 +3080,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -3004,7 +3088,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -3012,7 +3096,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -3020,7 +3104,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -3028,7 +3112,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -3036,7 +3120,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -3044,7 +3128,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -3052,7 +3136,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -3060,7 +3144,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -3068,7 +3152,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -3076,7 +3160,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -3084,7 +3168,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -3092,7 +3176,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -3100,7 +3184,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -3108,7 +3192,7 @@
         <v>80</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -3116,7 +3200,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -3124,7 +3208,7 @@
         <v>2</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -3132,7 +3216,7 @@
         <v>3</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -3140,7 +3224,7 @@
         <v>72</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -3148,7 +3232,7 @@
         <v>73</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -3156,7 +3240,7 @@
         <v>78</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -3185,7 +3269,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>74</v>

</xml_diff>